<commit_message>
adding tables / charts
</commit_message>
<xml_diff>
--- a/outputs/feb3/MAIN_feb3.xlsx
+++ b/outputs/feb3/MAIN_feb3.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edreiyu/Documents/Projects/vat_burden_analysis/outputs/feb3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA36966F-74EF-9842-8B6F-133F3BB494E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9BDE6F-54D2-DE49-9711-3F85D317E326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="2520" windowWidth="24180" windowHeight="17440" activeTab="4" xr2:uid="{30613F82-6F92-CA4A-972E-4B9F4D12BC37}"/>
+    <workbookView xWindow="760" yWindow="2640" windowWidth="35340" windowHeight="17440" activeTab="3" xr2:uid="{30613F82-6F92-CA4A-972E-4B9F4D12BC37}"/>
   </bookViews>
   <sheets>
     <sheet name="main_summary" sheetId="8" r:id="rId1"/>
     <sheet name="tax_share" sheetId="9" r:id="rId2"/>
     <sheet name="budget_share" sheetId="4" r:id="rId3"/>
-    <sheet name="exempt_by_category" sheetId="5" r:id="rId4"/>
-    <sheet name="tax_share_bydecile" sheetId="3" r:id="rId5"/>
-    <sheet name="vat_paid_and_foregone" sheetId="6" r:id="rId6"/>
-    <sheet name="senior_summary" sheetId="7" r:id="rId7"/>
-    <sheet name="xxmain_summary" sheetId="1" r:id="rId8"/>
-    <sheet name="xx-tax_share" sheetId="2" r:id="rId9"/>
+    <sheet name="tax_share_with_ratios" sheetId="10" r:id="rId4"/>
+    <sheet name="exempt_by_category" sheetId="5" r:id="rId5"/>
+    <sheet name="tax_share_bydecile" sheetId="3" r:id="rId6"/>
+    <sheet name="vat_paid_and_foregone" sheetId="6" r:id="rId7"/>
+    <sheet name="senior_summary" sheetId="7" r:id="rId8"/>
+    <sheet name="xxmain_summary" sheetId="1" r:id="rId9"/>
+    <sheet name="xx-tax_share" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="129">
   <si>
     <t>NPCINC</t>
   </si>
@@ -446,6 +447,27 @@
   <si>
     <t>VAT burden by Decile (In %)</t>
   </si>
+  <si>
+    <t>exempt_to_TOTALexpenditures</t>
+  </si>
+  <si>
+    <t>exempt_to_FIESexpenditures</t>
+  </si>
+  <si>
+    <t>exempt_to_income</t>
+  </si>
+  <si>
+    <t>vat_to_TOTALexpenditures</t>
+  </si>
+  <si>
+    <t>vat_to_FIESexpenditures</t>
+  </si>
+  <si>
+    <t>vat_to_income</t>
+  </si>
+  <si>
+    <t>estimated_vat_perHH</t>
+  </si>
 </sst>
 </file>
 
@@ -455,7 +477,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1026,7 +1048,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1071,14 +1093,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1090,6 +1112,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -1217,6 +1242,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-65B8-6341-98E9-04F4EC4F101B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1253,6 +1283,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-65B8-6341-98E9-04F4EC4F101B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1289,6 +1324,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-65B8-6341-98E9-04F4EC4F101B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1328,6 +1368,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-65B8-6341-98E9-04F4EC4F101B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1367,6 +1412,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-65B8-6341-98E9-04F4EC4F101B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -3479,6 +3529,472 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AA5D6B-21BD-1148-9FD5-75D290EA934C}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C2">
+        <v>32807166219.147499</v>
+      </c>
+      <c r="D2">
+        <v>29276373226.599098</v>
+      </c>
+      <c r="E2">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="F2">
+        <v>13799492511.298201</v>
+      </c>
+      <c r="G2">
+        <v>26530379528.095699</v>
+      </c>
+      <c r="H2">
+        <v>47.9860719795413</v>
+      </c>
+      <c r="I2">
+        <v>52.0139280204586</v>
+      </c>
+      <c r="J2">
+        <v>38.805201679891702</v>
+      </c>
+      <c r="K2">
+        <v>42.062433613191203</v>
+      </c>
+      <c r="L2">
+        <v>43.485191687715101</v>
+      </c>
+      <c r="M2">
+        <v>47.135252732605103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C3">
+        <v>41822410674.936996</v>
+      </c>
+      <c r="D3">
+        <v>35426039310.566101</v>
+      </c>
+      <c r="E3">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="F3">
+        <v>15540656739.6842</v>
+      </c>
+      <c r="G3">
+        <v>31712538484.6189</v>
+      </c>
+      <c r="H3">
+        <v>50.995229387828097</v>
+      </c>
+      <c r="I3">
+        <v>49.004770612171797</v>
+      </c>
+      <c r="J3">
+        <v>38.667980835992402</v>
+      </c>
+      <c r="K3">
+        <v>37.158682364039997</v>
+      </c>
+      <c r="L3">
+        <v>45.649703042336199</v>
+      </c>
+      <c r="M3">
+        <v>43.8678922118429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C4">
+        <v>47728594014.963997</v>
+      </c>
+      <c r="D4">
+        <v>39497871055.729301</v>
+      </c>
+      <c r="E4">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="F4">
+        <v>16596332039.166201</v>
+      </c>
+      <c r="G4">
+        <v>35088727599.755997</v>
+      </c>
+      <c r="H4">
+        <v>52.701812877131502</v>
+      </c>
+      <c r="I4">
+        <v>47.298187122868399</v>
+      </c>
+      <c r="J4">
+        <v>38.744899032207101</v>
+      </c>
+      <c r="K4">
+        <v>34.772304488925201</v>
+      </c>
+      <c r="L4">
+        <v>46.8187146960353</v>
+      </c>
+      <c r="M4">
+        <v>42.018295152540503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C5">
+        <v>55228987672.520798</v>
+      </c>
+      <c r="D5">
+        <v>44792749154.822098</v>
+      </c>
+      <c r="E5">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="F5">
+        <v>18343675668.4002</v>
+      </c>
+      <c r="G5">
+        <v>39517896410.847198</v>
+      </c>
+      <c r="H5">
+        <v>53.581345834579601</v>
+      </c>
+      <c r="I5">
+        <v>46.4186541654203</v>
+      </c>
+      <c r="J5">
+        <v>38.338962263800802</v>
+      </c>
+      <c r="K5">
+        <v>33.213854610496703</v>
+      </c>
+      <c r="L5">
+        <v>47.271536447249801</v>
+      </c>
+      <c r="M5">
+        <v>40.952332720184103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C6">
+        <v>62300009849.796898</v>
+      </c>
+      <c r="D6">
+        <v>49501029635.587097</v>
+      </c>
+      <c r="E6">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="F6">
+        <v>19654031599.593601</v>
+      </c>
+      <c r="G6">
+        <v>43456271435.610802</v>
+      </c>
+      <c r="H6">
+        <v>54.7728533758008</v>
+      </c>
+      <c r="I6">
+        <v>45.227146624199101</v>
+      </c>
+      <c r="J6">
+        <v>38.205836392969204</v>
+      </c>
+      <c r="K6">
+        <v>31.547397258810701</v>
+      </c>
+      <c r="L6">
+        <v>48.084332813362899</v>
+      </c>
+      <c r="M6">
+        <v>39.704288464868696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C7">
+        <v>70697712578.309692</v>
+      </c>
+      <c r="D7">
+        <v>54853430904.834999</v>
+      </c>
+      <c r="E7">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="F7">
+        <v>21273415620.797298</v>
+      </c>
+      <c r="G7">
+        <v>47787796098.107697</v>
+      </c>
+      <c r="H7">
+        <v>55.4835808348992</v>
+      </c>
+      <c r="I7">
+        <v>44.5164191651008</v>
+      </c>
+      <c r="J7">
+        <v>37.503873195248303</v>
+      </c>
+      <c r="K7">
+        <v>30.090670327181201</v>
+      </c>
+      <c r="L7">
+        <v>48.336776824972098</v>
+      </c>
+      <c r="M7">
+        <v>38.782288126524797</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C8">
+        <v>80541995781.497406</v>
+      </c>
+      <c r="D8">
+        <v>60962714759.237099</v>
+      </c>
+      <c r="E8">
+        <v>29745178079.321999</v>
+      </c>
+      <c r="F8">
+        <v>23156145640.561298</v>
+      </c>
+      <c r="G8">
+        <v>52901323719.883301</v>
+      </c>
+      <c r="H8">
+        <v>56.2276631050388</v>
+      </c>
+      <c r="I8">
+        <v>43.7723368949611</v>
+      </c>
+      <c r="J8">
+        <v>36.931265224688197</v>
+      </c>
+      <c r="K8">
+        <v>28.750399609393401</v>
+      </c>
+      <c r="L8">
+        <v>48.792410568978099</v>
+      </c>
+      <c r="M8">
+        <v>37.984111652528803</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C9">
+        <v>95316514865.332199</v>
+      </c>
+      <c r="D9">
+        <v>69592985603.748001</v>
+      </c>
+      <c r="E9">
+        <v>33990731017.6814</v>
+      </c>
+      <c r="F9">
+        <v>25837312021.747002</v>
+      </c>
+      <c r="G9">
+        <v>59828043039.428398</v>
+      </c>
+      <c r="H9">
+        <v>56.814044536406598</v>
+      </c>
+      <c r="I9">
+        <v>43.185955463593302</v>
+      </c>
+      <c r="J9">
+        <v>35.6609041630457</v>
+      </c>
+      <c r="K9">
+        <v>27.106857671255799</v>
+      </c>
+      <c r="L9">
+        <v>48.842179600138799</v>
+      </c>
+      <c r="M9">
+        <v>37.126316391799499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C10">
+        <v>117372854152.933</v>
+      </c>
+      <c r="D10">
+        <v>82061193028.969299</v>
+      </c>
+      <c r="E10">
+        <v>40157035542.102303</v>
+      </c>
+      <c r="F10">
+        <v>29129990531.2584</v>
+      </c>
+      <c r="G10">
+        <v>69287026073.360703</v>
+      </c>
+      <c r="H10">
+        <v>57.957510688341998</v>
+      </c>
+      <c r="I10">
+        <v>42.042489311658002</v>
+      </c>
+      <c r="J10">
+        <v>34.213222326330097</v>
+      </c>
+      <c r="K10">
+        <v>24.818337034986602</v>
+      </c>
+      <c r="L10">
+        <v>48.935476148788197</v>
+      </c>
+      <c r="M10">
+        <v>35.497888168619298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C11">
+        <v>205068163103.01001</v>
+      </c>
+      <c r="D11">
+        <v>124958992792.82401</v>
+      </c>
+      <c r="E11">
+        <v>60239542360.468002</v>
+      </c>
+      <c r="F11">
+        <v>40132550257.43</v>
+      </c>
+      <c r="G11">
+        <v>100372092617.89799</v>
+      </c>
+      <c r="H11">
+        <v>60.016226412446201</v>
+      </c>
+      <c r="I11">
+        <v>39.9837735875536</v>
+      </c>
+      <c r="J11">
+        <v>29.3753752161949</v>
+      </c>
+      <c r="K11">
+        <v>19.5703465863057</v>
+      </c>
+      <c r="L11">
+        <v>48.207448711067798</v>
+      </c>
+      <c r="M11">
+        <v>32.116576294726997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F725A2E-EC98-B848-9690-8DF0D559F542}">
   <dimension ref="A1:M15"/>
@@ -5670,6 +6186,1550 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B67FC65-0CFD-8945-8621-3D3C0A3AEE5E}">
+  <dimension ref="A1:U38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="12.1640625" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="8" customFormat="1" ht="51">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C2" s="2">
+        <v>32807166219.147499</v>
+      </c>
+      <c r="D2" s="2">
+        <v>29276373226.599098</v>
+      </c>
+      <c r="E2" s="2">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="F2" s="2">
+        <v>13799492511.298201</v>
+      </c>
+      <c r="G2" s="2">
+        <v>26530379528.095699</v>
+      </c>
+      <c r="H2" s="1">
+        <v>47.9860719795413</v>
+      </c>
+      <c r="I2" s="1">
+        <v>52.0139280204586</v>
+      </c>
+      <c r="J2" s="1">
+        <v>38.805201679891702</v>
+      </c>
+      <c r="K2" s="1">
+        <v>42.062433613191203</v>
+      </c>
+      <c r="L2" s="1">
+        <v>43.485191687715101</v>
+      </c>
+      <c r="M2" s="1">
+        <v>47.135252732605103</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1527706442.0157001</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1655939101.3557799</v>
+      </c>
+      <c r="P2" s="2">
+        <v>4.6566242015870101</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>5.2182230025258098</v>
+      </c>
+      <c r="R2" s="2">
+        <v>5.7583286375449498</v>
+      </c>
+      <c r="S2" s="2">
+        <v>5.0474920335829401</v>
+      </c>
+      <c r="T2" s="2">
+        <v>5.6562303279126196</v>
+      </c>
+      <c r="U2" s="2">
+        <v>6.2416713624550297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C3" s="2">
+        <v>41822410674.936996</v>
+      </c>
+      <c r="D3" s="2">
+        <v>35426039310.566101</v>
+      </c>
+      <c r="E3" s="2">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="F3" s="2">
+        <v>15540656739.6842</v>
+      </c>
+      <c r="G3" s="2">
+        <v>31712538484.6189</v>
+      </c>
+      <c r="H3" s="1">
+        <v>50.995229387828097</v>
+      </c>
+      <c r="I3" s="1">
+        <v>49.004770612171797</v>
+      </c>
+      <c r="J3" s="1">
+        <v>38.667980835992402</v>
+      </c>
+      <c r="K3" s="1">
+        <v>37.158682364039997</v>
+      </c>
+      <c r="L3" s="1">
+        <v>45.649703042336199</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43.8678922118429</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1940625809.3921599</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1864878808.7621</v>
+      </c>
+      <c r="P3" s="2">
+        <v>4.6401577003190901</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>5.47796436508035</v>
+      </c>
+      <c r="R3" s="2">
+        <v>6.11942752653938</v>
+      </c>
+      <c r="S3" s="2">
+        <v>4.4590418836848</v>
+      </c>
+      <c r="T3" s="2">
+        <v>5.26414706542114</v>
+      </c>
+      <c r="U3" s="2">
+        <v>5.8805724734606102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C4" s="2">
+        <v>47728594014.963997</v>
+      </c>
+      <c r="D4" s="2">
+        <v>39497871055.729301</v>
+      </c>
+      <c r="E4" s="2">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="F4" s="2">
+        <v>16596332039.166201</v>
+      </c>
+      <c r="G4" s="2">
+        <v>35088727599.755997</v>
+      </c>
+      <c r="H4" s="1">
+        <v>52.701812877131502</v>
+      </c>
+      <c r="I4" s="1">
+        <v>47.298187122868399</v>
+      </c>
+      <c r="J4" s="1">
+        <v>38.744899032207101</v>
+      </c>
+      <c r="K4" s="1">
+        <v>34.772304488925201</v>
+      </c>
+      <c r="L4" s="1">
+        <v>46.8187146960353</v>
+      </c>
+      <c r="M4" s="1">
+        <v>42.018295152540503</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2219087467.2707801</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1991559844.69994</v>
+      </c>
+      <c r="P4" s="2">
+        <v>4.6493878838648497</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>5.6182457635242402</v>
+      </c>
+      <c r="R4" s="2">
+        <v>6.3242175452557801</v>
+      </c>
+      <c r="S4" s="2">
+        <v>4.1726765386710198</v>
+      </c>
+      <c r="T4" s="2">
+        <v>5.0421954183048596</v>
+      </c>
+      <c r="U4" s="2">
+        <v>5.6757824547442102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C5" s="2">
+        <v>55228987672.520798</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44792749154.822098</v>
+      </c>
+      <c r="E5" s="2">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="F5" s="2">
+        <v>18343675668.4002</v>
+      </c>
+      <c r="G5" s="2">
+        <v>39517896410.847198</v>
+      </c>
+      <c r="H5" s="1">
+        <v>53.581345834579601</v>
+      </c>
+      <c r="I5" s="1">
+        <v>46.4186541654203</v>
+      </c>
+      <c r="J5" s="1">
+        <v>38.338962263800802</v>
+      </c>
+      <c r="K5" s="1">
+        <v>33.213854610496703</v>
+      </c>
+      <c r="L5" s="1">
+        <v>47.271536447249801</v>
+      </c>
+      <c r="M5" s="1">
+        <v>40.952332720184103</v>
+      </c>
+      <c r="N5" s="2">
+        <v>2540906489.0936298</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2201241080.2080202</v>
+      </c>
+      <c r="P5" s="2">
+        <v>4.60067547165609</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>5.6725843736699799</v>
+      </c>
+      <c r="R5" s="2">
+        <v>6.4297615001495503</v>
+      </c>
+      <c r="S5" s="2">
+        <v>3.9856625532595999</v>
+      </c>
+      <c r="T5" s="2">
+        <v>4.9142799264220898</v>
+      </c>
+      <c r="U5" s="2">
+        <v>5.57023849985044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C6" s="2">
+        <v>62300009849.796898</v>
+      </c>
+      <c r="D6" s="2">
+        <v>49501029635.587097</v>
+      </c>
+      <c r="E6" s="2">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="F6" s="2">
+        <v>19654031599.593601</v>
+      </c>
+      <c r="G6" s="2">
+        <v>43456271435.610802</v>
+      </c>
+      <c r="H6" s="1">
+        <v>54.7728533758008</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45.227146624199101</v>
+      </c>
+      <c r="J6" s="1">
+        <v>38.205836392969204</v>
+      </c>
+      <c r="K6" s="1">
+        <v>31.547397258810701</v>
+      </c>
+      <c r="L6" s="1">
+        <v>48.084332813362899</v>
+      </c>
+      <c r="M6" s="1">
+        <v>39.704288464868696</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2856268780.3220501</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2358483791.9512401</v>
+      </c>
+      <c r="P6" s="2">
+        <v>4.5847003671563096</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>5.7701199376035497</v>
+      </c>
+      <c r="R6" s="2">
+        <v>6.5727424050960996</v>
+      </c>
+      <c r="S6" s="2">
+        <v>3.78568767105729</v>
+      </c>
+      <c r="T6" s="2">
+        <v>4.7645146157842397</v>
+      </c>
+      <c r="U6" s="2">
+        <v>5.4272575949038897</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C7" s="2">
+        <v>70697712578.309692</v>
+      </c>
+      <c r="D7" s="2">
+        <v>54853430904.834999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="F7" s="2">
+        <v>21273415620.797298</v>
+      </c>
+      <c r="G7" s="2">
+        <v>47787796098.107697</v>
+      </c>
+      <c r="H7" s="1">
+        <v>55.4835808348992</v>
+      </c>
+      <c r="I7" s="1">
+        <v>44.5164191651008</v>
+      </c>
+      <c r="J7" s="1">
+        <v>37.503873195248303</v>
+      </c>
+      <c r="K7" s="1">
+        <v>30.090670327181201</v>
+      </c>
+      <c r="L7" s="1">
+        <v>48.336776824972098</v>
+      </c>
+      <c r="M7" s="1">
+        <v>38.782288126524797</v>
+      </c>
+      <c r="N7" s="2">
+        <v>3181725657.2772498</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2552809874.4956799</v>
+      </c>
+      <c r="P7" s="2">
+        <v>4.5004647834298002</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>5.8004132189966597</v>
+      </c>
+      <c r="R7" s="2">
+        <v>6.6580297001878996</v>
+      </c>
+      <c r="S7" s="2">
+        <v>3.61088043926175</v>
+      </c>
+      <c r="T7" s="2">
+        <v>4.6538745751829804</v>
+      </c>
+      <c r="U7" s="2">
+        <v>5.3419702998121004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C8" s="2">
+        <v>80541995781.497406</v>
+      </c>
+      <c r="D8" s="2">
+        <v>60962714759.237099</v>
+      </c>
+      <c r="E8" s="2">
+        <v>29745178079.321999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>23156145640.561298</v>
+      </c>
+      <c r="G8" s="2">
+        <v>52901323719.883301</v>
+      </c>
+      <c r="H8" s="1">
+        <v>56.2276631050388</v>
+      </c>
+      <c r="I8" s="1">
+        <v>43.7723368949611</v>
+      </c>
+      <c r="J8" s="1">
+        <v>36.931265224688197</v>
+      </c>
+      <c r="K8" s="1">
+        <v>28.750399609393401</v>
+      </c>
+      <c r="L8" s="1">
+        <v>48.792410568978099</v>
+      </c>
+      <c r="M8" s="1">
+        <v>37.984111652528803</v>
+      </c>
+      <c r="N8" s="2">
+        <v>3569421369.51864</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2778737476.8673501</v>
+      </c>
+      <c r="P8" s="2">
+        <v>4.4317518269625804</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>5.8550892682773696</v>
+      </c>
+      <c r="R8" s="2">
+        <v>6.7473195726046598</v>
+      </c>
+      <c r="S8" s="2">
+        <v>3.4500479531271999</v>
+      </c>
+      <c r="T8" s="2">
+        <v>4.5580933983034599</v>
+      </c>
+      <c r="U8" s="2">
+        <v>5.2526804273953296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C9" s="2">
+        <v>95316514865.332199</v>
+      </c>
+      <c r="D9" s="2">
+        <v>69592985603.748001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>33990731017.6814</v>
+      </c>
+      <c r="F9" s="2">
+        <v>25837312021.747002</v>
+      </c>
+      <c r="G9" s="2">
+        <v>59828043039.428398</v>
+      </c>
+      <c r="H9" s="1">
+        <v>56.814044536406598</v>
+      </c>
+      <c r="I9" s="1">
+        <v>43.185955463593302</v>
+      </c>
+      <c r="J9" s="1">
+        <v>35.6609041630457</v>
+      </c>
+      <c r="K9" s="1">
+        <v>27.106857671255799</v>
+      </c>
+      <c r="L9" s="1">
+        <v>48.842179600138799</v>
+      </c>
+      <c r="M9" s="1">
+        <v>37.126316391799499</v>
+      </c>
+      <c r="N9" s="2">
+        <v>4078887722.1217599</v>
+      </c>
+      <c r="O9" s="2">
+        <v>3100477442.6096401</v>
+      </c>
+      <c r="P9" s="2">
+        <v>4.2793084995654898</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>5.8610615520166602</v>
+      </c>
+      <c r="R9" s="2">
+        <v>6.8176853443687904</v>
+      </c>
+      <c r="S9" s="2">
+        <v>3.2528229205507002</v>
+      </c>
+      <c r="T9" s="2">
+        <v>4.45515796701594</v>
+      </c>
+      <c r="U9" s="2">
+        <v>5.1823146556311901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C10" s="2">
+        <v>117372854152.933</v>
+      </c>
+      <c r="D10" s="2">
+        <v>82061193028.969299</v>
+      </c>
+      <c r="E10" s="2">
+        <v>40157035542.102303</v>
+      </c>
+      <c r="F10" s="2">
+        <v>29129990531.2584</v>
+      </c>
+      <c r="G10" s="2">
+        <v>69287026073.360703</v>
+      </c>
+      <c r="H10" s="1">
+        <v>57.957510688341998</v>
+      </c>
+      <c r="I10" s="1">
+        <v>42.042489311658002</v>
+      </c>
+      <c r="J10" s="1">
+        <v>34.213222326330097</v>
+      </c>
+      <c r="K10" s="1">
+        <v>24.818337034986602</v>
+      </c>
+      <c r="L10" s="1">
+        <v>48.935476148788197</v>
+      </c>
+      <c r="M10" s="1">
+        <v>35.497888168619298</v>
+      </c>
+      <c r="N10" s="2">
+        <v>4818844265.0522804</v>
+      </c>
+      <c r="O10" s="2">
+        <v>3495598863.7509999</v>
+      </c>
+      <c r="P10" s="2">
+        <v>4.1055866791596101</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>5.8722571378545796</v>
+      </c>
+      <c r="R10" s="2">
+        <v>6.9549012826010399</v>
+      </c>
+      <c r="S10" s="2">
+        <v>2.9782004441984</v>
+      </c>
+      <c r="T10" s="2">
+        <v>4.25974658023432</v>
+      </c>
+      <c r="U10" s="2">
+        <v>5.0450987173989601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C11" s="2">
+        <v>205068163103.01001</v>
+      </c>
+      <c r="D11" s="2">
+        <v>124958992792.82401</v>
+      </c>
+      <c r="E11" s="2">
+        <v>60239542360.468002</v>
+      </c>
+      <c r="F11" s="2">
+        <v>40132550257.43</v>
+      </c>
+      <c r="G11" s="2">
+        <v>100372092617.89799</v>
+      </c>
+      <c r="H11" s="1">
+        <v>60.016226412446201</v>
+      </c>
+      <c r="I11" s="1">
+        <v>39.9837735875536</v>
+      </c>
+      <c r="J11" s="1">
+        <v>29.3753752161949</v>
+      </c>
+      <c r="K11" s="1">
+        <v>19.5703465863057</v>
+      </c>
+      <c r="L11" s="1">
+        <v>48.207448711067798</v>
+      </c>
+      <c r="M11" s="1">
+        <v>32.116576294726997</v>
+      </c>
+      <c r="N11" s="2">
+        <v>7228745083.2561598</v>
+      </c>
+      <c r="O11" s="2">
+        <v>4815906030.8915997</v>
+      </c>
+      <c r="P11" s="2">
+        <v>3.5250450259433799</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>5.7848938453281296</v>
+      </c>
+      <c r="R11" s="2">
+        <v>7.2019471694935504</v>
+      </c>
+      <c r="S11" s="2">
+        <v>2.34844159035669</v>
+      </c>
+      <c r="T11" s="2">
+        <v>3.8539891553672398</v>
+      </c>
+      <c r="U11" s="2">
+        <v>4.7980528305064398</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="34">
+      <c r="A16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C17" s="2">
+        <v>32807166219.147499</v>
+      </c>
+      <c r="D17" s="2">
+        <v>29276373226.599098</v>
+      </c>
+      <c r="E17" s="2">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="F17" s="2">
+        <v>13799492511.298201</v>
+      </c>
+      <c r="G17" s="2">
+        <v>26530379528.095699</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1527706442.0157001</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1655939101.3557799</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C18" s="2">
+        <v>41822410674.936996</v>
+      </c>
+      <c r="D18" s="2">
+        <v>35426039310.566101</v>
+      </c>
+      <c r="E18" s="2">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="F18" s="2">
+        <v>15540656739.6842</v>
+      </c>
+      <c r="G18" s="2">
+        <v>31712538484.6189</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1940625809.3921599</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1864878808.7621</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C19" s="2">
+        <v>47728594014.963997</v>
+      </c>
+      <c r="D19" s="2">
+        <v>39497871055.729301</v>
+      </c>
+      <c r="E19" s="2">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="F19" s="2">
+        <v>16596332039.166201</v>
+      </c>
+      <c r="G19" s="2">
+        <v>35088727599.755997</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2219087467.2707801</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1991559844.69994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C20" s="2">
+        <v>55228987672.520798</v>
+      </c>
+      <c r="D20" s="2">
+        <v>44792749154.822098</v>
+      </c>
+      <c r="E20" s="2">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="F20" s="2">
+        <v>18343675668.4002</v>
+      </c>
+      <c r="G20" s="2">
+        <v>39517896410.847198</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2540906489.0936298</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2201241080.2080202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C21" s="2">
+        <v>62300009849.796898</v>
+      </c>
+      <c r="D21" s="2">
+        <v>49501029635.587097</v>
+      </c>
+      <c r="E21" s="2">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="F21" s="2">
+        <v>19654031599.593601</v>
+      </c>
+      <c r="G21" s="2">
+        <v>43456271435.610802</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2856268780.3220501</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2358483791.9512401</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C22" s="2">
+        <v>70697712578.309692</v>
+      </c>
+      <c r="D22" s="2">
+        <v>54853430904.834999</v>
+      </c>
+      <c r="E22" s="2">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="F22" s="2">
+        <v>21273415620.797298</v>
+      </c>
+      <c r="G22" s="2">
+        <v>47787796098.107697</v>
+      </c>
+      <c r="H22" s="2">
+        <v>3181725657.2772498</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2552809874.4956799</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C23" s="2">
+        <v>80541995781.497406</v>
+      </c>
+      <c r="D23" s="2">
+        <v>60962714759.237099</v>
+      </c>
+      <c r="E23" s="2">
+        <v>29745178079.321999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>23156145640.561298</v>
+      </c>
+      <c r="G23" s="2">
+        <v>52901323719.883301</v>
+      </c>
+      <c r="H23" s="2">
+        <v>3569421369.51864</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2778737476.8673501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C24" s="2">
+        <v>95316514865.332199</v>
+      </c>
+      <c r="D24" s="2">
+        <v>69592985603.748001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>33990731017.6814</v>
+      </c>
+      <c r="F24" s="2">
+        <v>25837312021.747002</v>
+      </c>
+      <c r="G24" s="2">
+        <v>59828043039.428398</v>
+      </c>
+      <c r="H24" s="2">
+        <v>4078887722.1217599</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3100477442.6096401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C25" s="2">
+        <v>117372854152.933</v>
+      </c>
+      <c r="D25" s="2">
+        <v>82061193028.969299</v>
+      </c>
+      <c r="E25" s="2">
+        <v>40157035542.102303</v>
+      </c>
+      <c r="F25" s="2">
+        <v>29129990531.2584</v>
+      </c>
+      <c r="G25" s="2">
+        <v>69287026073.360703</v>
+      </c>
+      <c r="H25" s="2">
+        <v>4818844265.0522804</v>
+      </c>
+      <c r="I25" s="2">
+        <v>3495598863.7509999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C26" s="2">
+        <v>205068163103.01001</v>
+      </c>
+      <c r="D26" s="2">
+        <v>124958992792.82401</v>
+      </c>
+      <c r="E26" s="2">
+        <v>60239542360.468002</v>
+      </c>
+      <c r="F26" s="2">
+        <v>40132550257.43</v>
+      </c>
+      <c r="G26" s="2">
+        <v>100372092617.89799</v>
+      </c>
+      <c r="H26" s="2">
+        <v>7228745083.2561598</v>
+      </c>
+      <c r="I26" s="2">
+        <v>4815906030.8915997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="51">
+      <c r="A28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="K28" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C29" s="1">
+        <v>47.9860719795413</v>
+      </c>
+      <c r="D29" s="1">
+        <v>52.0139280204586</v>
+      </c>
+      <c r="E29" s="1">
+        <v>38.805201679891702</v>
+      </c>
+      <c r="F29" s="1">
+        <v>42.062433613191203</v>
+      </c>
+      <c r="G29" s="1">
+        <v>43.485191687715101</v>
+      </c>
+      <c r="H29" s="1">
+        <v>47.135252732605103</v>
+      </c>
+      <c r="I29" s="14">
+        <v>4.6566242015870101</v>
+      </c>
+      <c r="J29" s="1">
+        <v>5.2182230025258098</v>
+      </c>
+      <c r="K29" s="14">
+        <v>5.7583286375449498</v>
+      </c>
+      <c r="L29" s="1">
+        <v>5.0474920335829401</v>
+      </c>
+      <c r="M29" s="1">
+        <v>5.6562303279126196</v>
+      </c>
+      <c r="N29" s="1">
+        <v>6.2416713624550297</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C30" s="1">
+        <v>50.995229387828097</v>
+      </c>
+      <c r="D30" s="1">
+        <v>49.004770612171797</v>
+      </c>
+      <c r="E30" s="1">
+        <v>38.667980835992402</v>
+      </c>
+      <c r="F30" s="1">
+        <v>37.158682364039997</v>
+      </c>
+      <c r="G30" s="1">
+        <v>45.649703042336199</v>
+      </c>
+      <c r="H30" s="1">
+        <v>43.8678922118429</v>
+      </c>
+      <c r="I30" s="14">
+        <v>4.6401577003190901</v>
+      </c>
+      <c r="J30" s="1">
+        <v>5.47796436508035</v>
+      </c>
+      <c r="K30" s="14">
+        <v>6.11942752653938</v>
+      </c>
+      <c r="L30" s="1">
+        <v>4.4590418836848</v>
+      </c>
+      <c r="M30" s="1">
+        <v>5.26414706542114</v>
+      </c>
+      <c r="N30" s="1">
+        <v>5.8805724734606102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C31" s="1">
+        <v>52.701812877131502</v>
+      </c>
+      <c r="D31" s="1">
+        <v>47.298187122868399</v>
+      </c>
+      <c r="E31" s="1">
+        <v>38.744899032207101</v>
+      </c>
+      <c r="F31" s="1">
+        <v>34.772304488925201</v>
+      </c>
+      <c r="G31" s="1">
+        <v>46.8187146960353</v>
+      </c>
+      <c r="H31" s="1">
+        <v>42.018295152540503</v>
+      </c>
+      <c r="I31" s="14">
+        <v>4.6493878838648497</v>
+      </c>
+      <c r="J31" s="1">
+        <v>5.6182457635242402</v>
+      </c>
+      <c r="K31" s="14">
+        <v>6.3242175452557801</v>
+      </c>
+      <c r="L31" s="1">
+        <v>4.1726765386710198</v>
+      </c>
+      <c r="M31" s="1">
+        <v>5.0421954183048596</v>
+      </c>
+      <c r="N31" s="1">
+        <v>5.6757824547442102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C32" s="1">
+        <v>53.581345834579601</v>
+      </c>
+      <c r="D32" s="1">
+        <v>46.4186541654203</v>
+      </c>
+      <c r="E32" s="1">
+        <v>38.338962263800802</v>
+      </c>
+      <c r="F32" s="1">
+        <v>33.213854610496703</v>
+      </c>
+      <c r="G32" s="1">
+        <v>47.271536447249801</v>
+      </c>
+      <c r="H32" s="1">
+        <v>40.952332720184103</v>
+      </c>
+      <c r="I32" s="14">
+        <v>4.60067547165609</v>
+      </c>
+      <c r="J32" s="1">
+        <v>5.6725843736699799</v>
+      </c>
+      <c r="K32" s="14">
+        <v>6.4297615001495503</v>
+      </c>
+      <c r="L32" s="1">
+        <v>3.9856625532595999</v>
+      </c>
+      <c r="M32" s="1">
+        <v>4.9142799264220898</v>
+      </c>
+      <c r="N32" s="1">
+        <v>5.57023849985044</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C33" s="1">
+        <v>54.7728533758008</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45.227146624199101</v>
+      </c>
+      <c r="E33" s="1">
+        <v>38.205836392969204</v>
+      </c>
+      <c r="F33" s="1">
+        <v>31.547397258810701</v>
+      </c>
+      <c r="G33" s="1">
+        <v>48.084332813362899</v>
+      </c>
+      <c r="H33" s="1">
+        <v>39.704288464868696</v>
+      </c>
+      <c r="I33" s="14">
+        <v>4.5847003671563096</v>
+      </c>
+      <c r="J33" s="1">
+        <v>5.7701199376035497</v>
+      </c>
+      <c r="K33" s="14">
+        <v>6.5727424050960996</v>
+      </c>
+      <c r="L33" s="1">
+        <v>3.78568767105729</v>
+      </c>
+      <c r="M33" s="1">
+        <v>4.7645146157842397</v>
+      </c>
+      <c r="N33" s="1">
+        <v>5.4272575949038897</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C34" s="1">
+        <v>55.4835808348992</v>
+      </c>
+      <c r="D34" s="1">
+        <v>44.5164191651008</v>
+      </c>
+      <c r="E34" s="1">
+        <v>37.503873195248303</v>
+      </c>
+      <c r="F34" s="1">
+        <v>30.090670327181201</v>
+      </c>
+      <c r="G34" s="1">
+        <v>48.336776824972098</v>
+      </c>
+      <c r="H34" s="1">
+        <v>38.782288126524797</v>
+      </c>
+      <c r="I34" s="14">
+        <v>4.5004647834298002</v>
+      </c>
+      <c r="J34" s="1">
+        <v>5.8004132189966597</v>
+      </c>
+      <c r="K34" s="14">
+        <v>6.6580297001878996</v>
+      </c>
+      <c r="L34" s="1">
+        <v>3.61088043926175</v>
+      </c>
+      <c r="M34" s="1">
+        <v>4.6538745751829804</v>
+      </c>
+      <c r="N34" s="1">
+        <v>5.3419702998121004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C35" s="1">
+        <v>56.2276631050388</v>
+      </c>
+      <c r="D35" s="1">
+        <v>43.7723368949611</v>
+      </c>
+      <c r="E35" s="1">
+        <v>36.931265224688197</v>
+      </c>
+      <c r="F35" s="1">
+        <v>28.750399609393401</v>
+      </c>
+      <c r="G35" s="1">
+        <v>48.792410568978099</v>
+      </c>
+      <c r="H35" s="1">
+        <v>37.984111652528803</v>
+      </c>
+      <c r="I35" s="14">
+        <v>4.4317518269625804</v>
+      </c>
+      <c r="J35" s="1">
+        <v>5.8550892682773696</v>
+      </c>
+      <c r="K35" s="14">
+        <v>6.7473195726046598</v>
+      </c>
+      <c r="L35" s="1">
+        <v>3.4500479531271999</v>
+      </c>
+      <c r="M35" s="1">
+        <v>4.5580933983034599</v>
+      </c>
+      <c r="N35" s="1">
+        <v>5.2526804273953296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C36" s="1">
+        <v>56.814044536406598</v>
+      </c>
+      <c r="D36" s="1">
+        <v>43.185955463593302</v>
+      </c>
+      <c r="E36" s="1">
+        <v>35.6609041630457</v>
+      </c>
+      <c r="F36" s="1">
+        <v>27.106857671255799</v>
+      </c>
+      <c r="G36" s="1">
+        <v>48.842179600138799</v>
+      </c>
+      <c r="H36" s="1">
+        <v>37.126316391799499</v>
+      </c>
+      <c r="I36" s="14">
+        <v>4.2793084995654898</v>
+      </c>
+      <c r="J36" s="1">
+        <v>5.8610615520166602</v>
+      </c>
+      <c r="K36" s="14">
+        <v>6.8176853443687904</v>
+      </c>
+      <c r="L36" s="1">
+        <v>3.2528229205507002</v>
+      </c>
+      <c r="M36" s="1">
+        <v>4.45515796701594</v>
+      </c>
+      <c r="N36" s="1">
+        <v>5.1823146556311901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C37" s="1">
+        <v>57.957510688341998</v>
+      </c>
+      <c r="D37" s="1">
+        <v>42.042489311658002</v>
+      </c>
+      <c r="E37" s="1">
+        <v>34.213222326330097</v>
+      </c>
+      <c r="F37" s="1">
+        <v>24.818337034986602</v>
+      </c>
+      <c r="G37" s="1">
+        <v>48.935476148788197</v>
+      </c>
+      <c r="H37" s="1">
+        <v>35.497888168619298</v>
+      </c>
+      <c r="I37" s="14">
+        <v>4.1055866791596101</v>
+      </c>
+      <c r="J37" s="1">
+        <v>5.8722571378545796</v>
+      </c>
+      <c r="K37" s="14">
+        <v>6.9549012826010399</v>
+      </c>
+      <c r="L37" s="1">
+        <v>2.9782004441984</v>
+      </c>
+      <c r="M37" s="1">
+        <v>4.25974658023432</v>
+      </c>
+      <c r="N37" s="1">
+        <v>5.0450987173989601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38">
+        <v>10</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C38" s="1">
+        <v>60.016226412446201</v>
+      </c>
+      <c r="D38" s="1">
+        <v>39.9837735875536</v>
+      </c>
+      <c r="E38" s="1">
+        <v>29.3753752161949</v>
+      </c>
+      <c r="F38" s="1">
+        <v>19.5703465863057</v>
+      </c>
+      <c r="G38" s="1">
+        <v>48.207448711067798</v>
+      </c>
+      <c r="H38" s="1">
+        <v>32.116576294726997</v>
+      </c>
+      <c r="I38" s="14">
+        <v>3.5250450259433799</v>
+      </c>
+      <c r="J38" s="1">
+        <v>5.7848938453281296</v>
+      </c>
+      <c r="K38" s="14">
+        <v>7.2019471694935504</v>
+      </c>
+      <c r="L38" s="1">
+        <v>2.34844159035669</v>
+      </c>
+      <c r="M38" s="1">
+        <v>3.8539891553672398</v>
+      </c>
+      <c r="N38" s="1">
+        <v>4.7980528305064398</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61A1F9D-EB5B-1C46-BEE0-9C566D64DA42}">
   <dimension ref="A1:U24"/>
   <sheetViews>
@@ -6597,11 +8657,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA719825-5205-FE4C-B220-F0E805A976AA}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L23" sqref="L22:L23"/>
     </sheetView>
   </sheetViews>
@@ -7394,7 +9454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2835AA48-B8D0-BB4F-9D44-004653D39453}">
   <dimension ref="A1:R11"/>
   <sheetViews>
@@ -8035,7 +10095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79482C87-9E54-3145-A88B-A07A29DD7EB7}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -8468,7 +10528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EEC793-A1C4-FF48-AB6B-B60CEDF4D66E}">
   <dimension ref="A1:K15"/>
   <sheetViews>
@@ -8941,470 +11001,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AA5D6B-21BD-1148-9FD5-75D290EA934C}">
-  <dimension ref="A1:M11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2747642.50515944</v>
-      </c>
-      <c r="C2">
-        <v>32807166219.147499</v>
-      </c>
-      <c r="D2">
-        <v>29276373226.599098</v>
-      </c>
-      <c r="E2">
-        <v>12730887016.797501</v>
-      </c>
-      <c r="F2">
-        <v>13799492511.298201</v>
-      </c>
-      <c r="G2">
-        <v>26530379528.095699</v>
-      </c>
-      <c r="H2">
-        <v>47.9860719795413</v>
-      </c>
-      <c r="I2">
-        <v>52.0139280204586</v>
-      </c>
-      <c r="J2">
-        <v>38.805201679891702</v>
-      </c>
-      <c r="K2">
-        <v>42.062433613191203</v>
-      </c>
-      <c r="L2">
-        <v>43.485191687715101</v>
-      </c>
-      <c r="M2">
-        <v>47.135252732605103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2748295.6540946802</v>
-      </c>
-      <c r="C3">
-        <v>41822410674.936996</v>
-      </c>
-      <c r="D3">
-        <v>35426039310.566101</v>
-      </c>
-      <c r="E3">
-        <v>16171881744.9347</v>
-      </c>
-      <c r="F3">
-        <v>15540656739.6842</v>
-      </c>
-      <c r="G3">
-        <v>31712538484.6189</v>
-      </c>
-      <c r="H3">
-        <v>50.995229387828097</v>
-      </c>
-      <c r="I3">
-        <v>49.004770612171797</v>
-      </c>
-      <c r="J3">
-        <v>38.667980835992402</v>
-      </c>
-      <c r="K3">
-        <v>37.158682364039997</v>
-      </c>
-      <c r="L3">
-        <v>45.649703042336199</v>
-      </c>
-      <c r="M3">
-        <v>43.8678922118429</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2747874.69444041</v>
-      </c>
-      <c r="C4">
-        <v>47728594014.963997</v>
-      </c>
-      <c r="D4">
-        <v>39497871055.729301</v>
-      </c>
-      <c r="E4">
-        <v>18492395560.589802</v>
-      </c>
-      <c r="F4">
-        <v>16596332039.166201</v>
-      </c>
-      <c r="G4">
-        <v>35088727599.755997</v>
-      </c>
-      <c r="H4">
-        <v>52.701812877131502</v>
-      </c>
-      <c r="I4">
-        <v>47.298187122868399</v>
-      </c>
-      <c r="J4">
-        <v>38.744899032207101</v>
-      </c>
-      <c r="K4">
-        <v>34.772304488925201</v>
-      </c>
-      <c r="L4">
-        <v>46.8187146960353</v>
-      </c>
-      <c r="M4">
-        <v>42.018295152540503</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>2747979.4784429399</v>
-      </c>
-      <c r="C5">
-        <v>55228987672.520798</v>
-      </c>
-      <c r="D5">
-        <v>44792749154.822098</v>
-      </c>
-      <c r="E5">
-        <v>21174220742.446899</v>
-      </c>
-      <c r="F5">
-        <v>18343675668.4002</v>
-      </c>
-      <c r="G5">
-        <v>39517896410.847198</v>
-      </c>
-      <c r="H5">
-        <v>53.581345834579601</v>
-      </c>
-      <c r="I5">
-        <v>46.4186541654203</v>
-      </c>
-      <c r="J5">
-        <v>38.338962263800802</v>
-      </c>
-      <c r="K5">
-        <v>33.213854610496703</v>
-      </c>
-      <c r="L5">
-        <v>47.271536447249801</v>
-      </c>
-      <c r="M5">
-        <v>40.952332720184103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2747628.8515828899</v>
-      </c>
-      <c r="C6">
-        <v>62300009849.796898</v>
-      </c>
-      <c r="D6">
-        <v>49501029635.587097</v>
-      </c>
-      <c r="E6">
-        <v>23802239836.017101</v>
-      </c>
-      <c r="F6">
-        <v>19654031599.593601</v>
-      </c>
-      <c r="G6">
-        <v>43456271435.610802</v>
-      </c>
-      <c r="H6">
-        <v>54.7728533758008</v>
-      </c>
-      <c r="I6">
-        <v>45.227146624199101</v>
-      </c>
-      <c r="J6">
-        <v>38.205836392969204</v>
-      </c>
-      <c r="K6">
-        <v>31.547397258810701</v>
-      </c>
-      <c r="L6">
-        <v>48.084332813362899</v>
-      </c>
-      <c r="M6">
-        <v>39.704288464868696</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2748336.9317767601</v>
-      </c>
-      <c r="C7">
-        <v>70697712578.309692</v>
-      </c>
-      <c r="D7">
-        <v>54853430904.834999</v>
-      </c>
-      <c r="E7">
-        <v>26514380477.310398</v>
-      </c>
-      <c r="F7">
-        <v>21273415620.797298</v>
-      </c>
-      <c r="G7">
-        <v>47787796098.107697</v>
-      </c>
-      <c r="H7">
-        <v>55.4835808348992</v>
-      </c>
-      <c r="I7">
-        <v>44.5164191651008</v>
-      </c>
-      <c r="J7">
-        <v>37.503873195248303</v>
-      </c>
-      <c r="K7">
-        <v>30.090670327181201</v>
-      </c>
-      <c r="L7">
-        <v>48.336776824972098</v>
-      </c>
-      <c r="M7">
-        <v>38.782288126524797</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>2747846.3569293302</v>
-      </c>
-      <c r="C8">
-        <v>80541995781.497406</v>
-      </c>
-      <c r="D8">
-        <v>60962714759.237099</v>
-      </c>
-      <c r="E8">
-        <v>29745178079.321999</v>
-      </c>
-      <c r="F8">
-        <v>23156145640.561298</v>
-      </c>
-      <c r="G8">
-        <v>52901323719.883301</v>
-      </c>
-      <c r="H8">
-        <v>56.2276631050388</v>
-      </c>
-      <c r="I8">
-        <v>43.7723368949611</v>
-      </c>
-      <c r="J8">
-        <v>36.931265224688197</v>
-      </c>
-      <c r="K8">
-        <v>28.750399609393401</v>
-      </c>
-      <c r="L8">
-        <v>48.792410568978099</v>
-      </c>
-      <c r="M8">
-        <v>37.984111652528803</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>2747984.4327531499</v>
-      </c>
-      <c r="C9">
-        <v>95316514865.332199</v>
-      </c>
-      <c r="D9">
-        <v>69592985603.748001</v>
-      </c>
-      <c r="E9">
-        <v>33990731017.6814</v>
-      </c>
-      <c r="F9">
-        <v>25837312021.747002</v>
-      </c>
-      <c r="G9">
-        <v>59828043039.428398</v>
-      </c>
-      <c r="H9">
-        <v>56.814044536406598</v>
-      </c>
-      <c r="I9">
-        <v>43.185955463593302</v>
-      </c>
-      <c r="J9">
-        <v>35.6609041630457</v>
-      </c>
-      <c r="K9">
-        <v>27.106857671255799</v>
-      </c>
-      <c r="L9">
-        <v>48.842179600138799</v>
-      </c>
-      <c r="M9">
-        <v>37.126316391799499</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>2748042.5822946099</v>
-      </c>
-      <c r="C10">
-        <v>117372854152.933</v>
-      </c>
-      <c r="D10">
-        <v>82061193028.969299</v>
-      </c>
-      <c r="E10">
-        <v>40157035542.102303</v>
-      </c>
-      <c r="F10">
-        <v>29129990531.2584</v>
-      </c>
-      <c r="G10">
-        <v>69287026073.360703</v>
-      </c>
-      <c r="H10">
-        <v>57.957510688341998</v>
-      </c>
-      <c r="I10">
-        <v>42.042489311658002</v>
-      </c>
-      <c r="J10">
-        <v>34.213222326330097</v>
-      </c>
-      <c r="K10">
-        <v>24.818337034986602</v>
-      </c>
-      <c r="L10">
-        <v>48.935476148788197</v>
-      </c>
-      <c r="M10">
-        <v>35.497888168619298</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>2748063.5193039002</v>
-      </c>
-      <c r="C11">
-        <v>205068163103.01001</v>
-      </c>
-      <c r="D11">
-        <v>124958992792.82401</v>
-      </c>
-      <c r="E11">
-        <v>60239542360.468002</v>
-      </c>
-      <c r="F11">
-        <v>40132550257.43</v>
-      </c>
-      <c r="G11">
-        <v>100372092617.89799</v>
-      </c>
-      <c r="H11">
-        <v>60.016226412446201</v>
-      </c>
-      <c r="I11">
-        <v>39.9837735875536</v>
-      </c>
-      <c r="J11">
-        <v>29.3753752161949</v>
-      </c>
-      <c r="K11">
-        <v>19.5703465863057</v>
-      </c>
-      <c r="L11">
-        <v>48.207448711067798</v>
-      </c>
-      <c r="M11">
-        <v>32.116576294726997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
private educ and health
</commit_message>
<xml_diff>
--- a/outputs/feb3/MAIN_feb3.xlsx
+++ b/outputs/feb3/MAIN_feb3.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edreiyu/Documents/Projects/vat_burden_analysis/outputs/feb3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9BDE6F-54D2-DE49-9711-3F85D317E326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FEEF43-32D7-2349-A360-449AFF82094F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="2640" windowWidth="35340" windowHeight="17440" activeTab="3" xr2:uid="{30613F82-6F92-CA4A-972E-4B9F4D12BC37}"/>
+    <workbookView xWindow="5540" yWindow="2120" windowWidth="27880" windowHeight="17440" activeTab="4" xr2:uid="{30613F82-6F92-CA4A-972E-4B9F4D12BC37}"/>
   </bookViews>
   <sheets>
     <sheet name="main_summary" sheetId="8" r:id="rId1"/>
     <sheet name="tax_share" sheetId="9" r:id="rId2"/>
     <sheet name="budget_share" sheetId="4" r:id="rId3"/>
     <sheet name="tax_share_with_ratios" sheetId="10" r:id="rId4"/>
-    <sheet name="exempt_by_category" sheetId="5" r:id="rId5"/>
-    <sheet name="tax_share_bydecile" sheetId="3" r:id="rId6"/>
-    <sheet name="vat_paid_and_foregone" sheetId="6" r:id="rId7"/>
-    <sheet name="senior_summary" sheetId="7" r:id="rId8"/>
-    <sheet name="xxmain_summary" sheetId="1" r:id="rId9"/>
-    <sheet name="xx-tax_share" sheetId="2" r:id="rId10"/>
+    <sheet name="exempt_educ_health" sheetId="11" r:id="rId5"/>
+    <sheet name="exempt_by_category" sheetId="5" r:id="rId6"/>
+    <sheet name="tax_share_bydecile" sheetId="3" r:id="rId7"/>
+    <sheet name="vat_paid_and_foregone" sheetId="6" r:id="rId8"/>
+    <sheet name="senior_summary" sheetId="7" r:id="rId9"/>
+    <sheet name="xxmain_summary" sheetId="1" r:id="rId10"/>
+    <sheet name="xx-tax_share" sheetId="2" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="149">
   <si>
     <t>NPCINC</t>
   </si>
@@ -468,6 +469,66 @@
   <si>
     <t>estimated_vat_perHH</t>
   </si>
+  <si>
+    <t>vat_total_educ_health</t>
+  </si>
+  <si>
+    <t>vat_private_health</t>
+  </si>
+  <si>
+    <t>vat_medicines</t>
+  </si>
+  <si>
+    <t>vat_private_educ</t>
+  </si>
+  <si>
+    <t>total_educ_health_share_HHexp</t>
+  </si>
+  <si>
+    <t>private_health_share_HHexp</t>
+  </si>
+  <si>
+    <t>medicines_share_HHexp</t>
+  </si>
+  <si>
+    <t>private_educ_share_HHexp</t>
+  </si>
+  <si>
+    <t>total_educ_health_share_income</t>
+  </si>
+  <si>
+    <t>private_health_share_income</t>
+  </si>
+  <si>
+    <t>medicines_share_income</t>
+  </si>
+  <si>
+    <t>private_educ_share_income</t>
+  </si>
+  <si>
+    <t>total_educ_health_share_exp</t>
+  </si>
+  <si>
+    <t>private_health_share_exp</t>
+  </si>
+  <si>
+    <t>medicines_share_exp</t>
+  </si>
+  <si>
+    <t>private_educ_share_exp</t>
+  </si>
+  <si>
+    <t>total_educ_health_expenditures</t>
+  </si>
+  <si>
+    <t>private_health_expenditures</t>
+  </si>
+  <si>
+    <t>medicines_expenditures</t>
+  </si>
+  <si>
+    <t>private_educ_expenditures</t>
+  </si>
 </sst>
 </file>
 
@@ -479,7 +540,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -675,6 +736,13 @@
       <color rgb="FF222222"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1048,7 +1116,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1115,6 +1183,9 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="26" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="28" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -3530,6 +3601,481 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EEC793-A1C4-FF48-AB6B-B60CEDF4D66E}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" customWidth="1"/>
+    <col min="6" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C2" s="2">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="D2" s="2">
+        <v>13799492511.298201</v>
+      </c>
+      <c r="E2" s="2">
+        <v>26530379528.095699</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1527706442.0157001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1655939101.3557799</v>
+      </c>
+      <c r="H2" s="1">
+        <v>5.7081655079756999</v>
+      </c>
+      <c r="I2" s="1">
+        <v>6.2918344920242903</v>
+      </c>
+      <c r="J2" s="1">
+        <v>5.7583286375449596</v>
+      </c>
+      <c r="K2" s="1">
+        <v>6.2416713624550297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C3" s="2">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="D3" s="2">
+        <v>15540656739.6842</v>
+      </c>
+      <c r="E3" s="2">
+        <v>31712538484.6189</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1940625809.3921599</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1864878808.7621</v>
+      </c>
+      <c r="H3" s="1">
+        <v>6.0303049401519999</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5.9696950598479903</v>
+      </c>
+      <c r="J3" s="1">
+        <v>6.11942752653938</v>
+      </c>
+      <c r="K3" s="1">
+        <v>5.8805724734606102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C4" s="2">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="D4" s="2">
+        <v>16596332039.166201</v>
+      </c>
+      <c r="E4" s="2">
+        <v>35088727599.755997</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2219087467.2707801</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1991559844.69994</v>
+      </c>
+      <c r="H4" s="1">
+        <v>6.1898610711613902</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5.8101389288386098</v>
+      </c>
+      <c r="J4" s="1">
+        <v>6.3242175452557801</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5.6757824547442102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C5" s="2">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="D5" s="2">
+        <v>18343675668.4002</v>
+      </c>
+      <c r="E5" s="2">
+        <v>39517896410.847198</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2540906489.0936298</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2201241080.2080202</v>
+      </c>
+      <c r="H5" s="1">
+        <v>6.2902942340410304</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5.7097057659589598</v>
+      </c>
+      <c r="J5" s="1">
+        <v>6.4297615001495503</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5.57023849985044</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C6" s="2">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="D6" s="2">
+        <v>19654031599.593601</v>
+      </c>
+      <c r="E6" s="2">
+        <v>43456271435.610802</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2856268780.3220501</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2358483791.9512401</v>
+      </c>
+      <c r="H6" s="1">
+        <v>6.4047799708266</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5.5952200291733902</v>
+      </c>
+      <c r="J6" s="1">
+        <v>6.5727424050960996</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5.4272575949038897</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C7" s="2">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="D7" s="2">
+        <v>21273415620.797298</v>
+      </c>
+      <c r="E7" s="2">
+        <v>47787796098.107697</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3181725657.2772498</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2552809874.4956799</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6.4988720176579404</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5.5011279823420498</v>
+      </c>
+      <c r="J7" s="1">
+        <v>6.6580297001878996</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5.3419702998121004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C8" s="2">
+        <v>29745178079.321999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>23156145640.561298</v>
+      </c>
+      <c r="E8" s="2">
+        <v>52901323719.883301</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3569421369.51863</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2778737476.8673501</v>
+      </c>
+      <c r="H8" s="1">
+        <v>6.62365764514223</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5.3763423548577602</v>
+      </c>
+      <c r="J8" s="1">
+        <v>6.7473195726046598</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5.2526804273953296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C9" s="2">
+        <v>33990731017.6814</v>
+      </c>
+      <c r="D9" s="2">
+        <v>25837312021.747002</v>
+      </c>
+      <c r="E9" s="2">
+        <v>59828043039.428398</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4078887722.1217699</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3100477442.6096401</v>
+      </c>
+      <c r="H9" s="1">
+        <v>6.7137976077127703</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5.2862023922872199</v>
+      </c>
+      <c r="J9" s="1">
+        <v>6.8176853443688001</v>
+      </c>
+      <c r="K9" s="1">
+        <v>5.1823146556311901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C10" s="2">
+        <v>40157035542.102303</v>
+      </c>
+      <c r="D10" s="2">
+        <v>29129990531.2584</v>
+      </c>
+      <c r="E10" s="2">
+        <v>69287026073.360703</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4818844265.0522804</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3495598863.7510099</v>
+      </c>
+      <c r="H10" s="1">
+        <v>6.8620584936718902</v>
+      </c>
+      <c r="I10" s="1">
+        <v>5.1379415063281</v>
+      </c>
+      <c r="J10" s="1">
+        <v>6.9549012826010399</v>
+      </c>
+      <c r="K10" s="1">
+        <v>5.0450987173989601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C11" s="2">
+        <v>60239542360.468002</v>
+      </c>
+      <c r="D11" s="2">
+        <v>40132550257.43</v>
+      </c>
+      <c r="E11" s="2">
+        <v>100372092617.89799</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7228745083.2561598</v>
+      </c>
+      <c r="G11" s="2">
+        <v>4815906030.8915997</v>
+      </c>
+      <c r="H11" s="1">
+        <v>7.1193827019703901</v>
+      </c>
+      <c r="I11" s="1">
+        <v>4.8806172980296099</v>
+      </c>
+      <c r="J11" s="1">
+        <v>7.2019471694935504</v>
+      </c>
+      <c r="K11" s="1">
+        <v>4.7980528305064398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1">
+      <c r="A12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" ref="B12:G12" si="0">SUM(B2:B11)</f>
+        <v>27479695.00677811</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>283018492377.6701</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>223463602629.93637</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>506482095007.60669</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>33962219085.320412</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>26815632315.592361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="C13" s="6">
+        <f>C12/E12</f>
+        <v>0.558792690141237</v>
+      </c>
+      <c r="D13" s="6">
+        <f>D12/E12</f>
+        <v>0.44120730985876261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="C14" s="3">
+        <f>C12*12</f>
+        <v>3396221908532.041</v>
+      </c>
+      <c r="D14" s="3">
+        <f>D12*12</f>
+        <v>2681563231559.2363</v>
+      </c>
+      <c r="E14" s="3">
+        <f>E12*12</f>
+        <v>6077785140091.2803</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="C15" s="3">
+        <f>C14*0.12</f>
+        <v>407546629023.84491</v>
+      </c>
+      <c r="D15" s="3">
+        <f>D14*0.12</f>
+        <v>321787587787.10834</v>
+      </c>
+      <c r="E15" s="3">
+        <f>E14*0.12</f>
+        <v>729334216810.95361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AA5D6B-21BD-1148-9FD5-75D290EA934C}">
   <dimension ref="A1:M11"/>
   <sheetViews>
@@ -6189,7 +6735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B67FC65-0CFD-8945-8621-3D3C0A3AEE5E}">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -7730,6 +8276,1112 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BAFD56-773F-394D-B79D-7324C3405722}">
+  <dimension ref="A1:AB14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" s="8" customFormat="1" ht="51">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="M1" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="N1" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2747642.50515944</v>
+      </c>
+      <c r="C2" s="2">
+        <v>32807166219.147499</v>
+      </c>
+      <c r="D2" s="2">
+        <v>29276373226.599098</v>
+      </c>
+      <c r="E2" s="2">
+        <v>12730887016.797501</v>
+      </c>
+      <c r="F2" s="2">
+        <v>13799492511.298201</v>
+      </c>
+      <c r="G2" s="2">
+        <v>26530379528.095699</v>
+      </c>
+      <c r="H2" s="2">
+        <v>73210301.349811703</v>
+      </c>
+      <c r="I2" s="2">
+        <v>61712897.949039899</v>
+      </c>
+      <c r="J2" s="2">
+        <v>34967024.708207801</v>
+      </c>
+      <c r="K2" s="2">
+        <v>169890224.00705901</v>
+      </c>
+      <c r="L2" s="45">
+        <v>0.27594894099528999</v>
+      </c>
+      <c r="M2" s="45">
+        <v>0.23261219419679099</v>
+      </c>
+      <c r="N2" s="45">
+        <v>0.13179994153938701</v>
+      </c>
+      <c r="O2" s="45">
+        <v>0.64036107673146903</v>
+      </c>
+      <c r="P2" s="32">
+        <v>0.223153383199196</v>
+      </c>
+      <c r="Q2" s="32">
+        <v>0.18810798085029901</v>
+      </c>
+      <c r="R2" s="32">
+        <v>0.10658349604056799</v>
+      </c>
+      <c r="S2" s="32">
+        <v>0.51784486009006403</v>
+      </c>
+      <c r="T2" s="32">
+        <v>0.25006615670309901</v>
+      </c>
+      <c r="U2" s="32">
+        <v>0.21079420415698999</v>
+      </c>
+      <c r="V2" s="32">
+        <v>0.11943769276871501</v>
+      </c>
+      <c r="W2" s="32">
+        <v>0.58029805362880604</v>
+      </c>
+      <c r="X2" s="2">
+        <v>8785236.1619773991</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>7405547.7538847905</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>4196042.9649849404</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>20386826.8808471</v>
+      </c>
+      <c r="AB2" s="33">
+        <f>AA2/$AA$12</f>
+        <v>9.8937849133188607E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2748295.6540946802</v>
+      </c>
+      <c r="C3" s="2">
+        <v>41822410674.936996</v>
+      </c>
+      <c r="D3" s="2">
+        <v>35426039310.566101</v>
+      </c>
+      <c r="E3" s="2">
+        <v>16171881744.9347</v>
+      </c>
+      <c r="F3" s="2">
+        <v>15540656739.6842</v>
+      </c>
+      <c r="G3" s="2">
+        <v>31712538484.6189</v>
+      </c>
+      <c r="H3" s="2">
+        <v>129638745.142389</v>
+      </c>
+      <c r="I3" s="2">
+        <v>117888631.371511</v>
+      </c>
+      <c r="J3" s="2">
+        <v>44173461.526427902</v>
+      </c>
+      <c r="K3" s="2">
+        <v>291700838.04032898</v>
+      </c>
+      <c r="L3" s="45">
+        <v>0.40879333959741598</v>
+      </c>
+      <c r="M3" s="45">
+        <v>0.37174139001420098</v>
+      </c>
+      <c r="N3" s="45">
+        <v>0.13929336356297201</v>
+      </c>
+      <c r="O3" s="45">
+        <v>0.91982809317459002</v>
+      </c>
+      <c r="P3" s="32">
+        <v>0.30997434880069802</v>
+      </c>
+      <c r="Q3" s="32">
+        <v>0.28187909178118697</v>
+      </c>
+      <c r="R3" s="32">
+        <v>0.105621509648892</v>
+      </c>
+      <c r="S3" s="32">
+        <v>0.69747495023077799</v>
+      </c>
+      <c r="T3" s="32">
+        <v>0.36594196716685701</v>
+      </c>
+      <c r="U3" s="32">
+        <v>0.33277395290517198</v>
+      </c>
+      <c r="V3" s="32">
+        <v>0.124692069410234</v>
+      </c>
+      <c r="W3" s="32">
+        <v>0.82340798948226401</v>
+      </c>
+      <c r="X3" s="2">
+        <v>15556649.4170867</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>14146635.7645813</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>5300815.3831713498</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>35004100.5648394</v>
+      </c>
+      <c r="AB3" s="33">
+        <f t="shared" ref="AB3:AB12" si="0">AA3/$AA$12</f>
+        <v>1.6987589294637406E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2747874.69444041</v>
+      </c>
+      <c r="C4" s="2">
+        <v>47728594014.963997</v>
+      </c>
+      <c r="D4" s="2">
+        <v>39497871055.729301</v>
+      </c>
+      <c r="E4" s="2">
+        <v>18492395560.589802</v>
+      </c>
+      <c r="F4" s="2">
+        <v>16596332039.166201</v>
+      </c>
+      <c r="G4" s="2">
+        <v>35088727599.755997</v>
+      </c>
+      <c r="H4" s="2">
+        <v>192009650.98493901</v>
+      </c>
+      <c r="I4" s="2">
+        <v>153593294.110075</v>
+      </c>
+      <c r="J4" s="2">
+        <v>65869647.788779497</v>
+      </c>
+      <c r="K4" s="2">
+        <v>411472592.883793</v>
+      </c>
+      <c r="L4" s="45">
+        <v>0.54721178030483397</v>
+      </c>
+      <c r="M4" s="45">
+        <v>0.437728309393421</v>
+      </c>
+      <c r="N4" s="45">
+        <v>0.18772310167564299</v>
+      </c>
+      <c r="O4" s="45">
+        <v>1.1726631913738901</v>
+      </c>
+      <c r="P4" s="32">
+        <v>0.40229479821831599</v>
+      </c>
+      <c r="Q4" s="32">
+        <v>0.32180561208637298</v>
+      </c>
+      <c r="R4" s="32">
+        <v>0.13800877471506401</v>
+      </c>
+      <c r="S4" s="32">
+        <v>0.86210918501975498</v>
+      </c>
+      <c r="T4" s="32">
+        <v>0.48612658316197299</v>
+      </c>
+      <c r="U4" s="32">
+        <v>0.38886474132583798</v>
+      </c>
+      <c r="V4" s="32">
+        <v>0.16676759032364299</v>
+      </c>
+      <c r="W4" s="32">
+        <v>1.0417589148114501</v>
+      </c>
+      <c r="X4" s="2">
+        <v>23041158.118192598</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>18431195.293209001</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>7904357.73465354</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>49376711.146055199</v>
+      </c>
+      <c r="AB4" s="33">
+        <f t="shared" si="0"/>
+        <v>2.3962657978181909E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2747979.4784429399</v>
+      </c>
+      <c r="C5" s="2">
+        <v>55228987672.520798</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44792749154.822098</v>
+      </c>
+      <c r="E5" s="2">
+        <v>21174220742.446899</v>
+      </c>
+      <c r="F5" s="2">
+        <v>18343675668.4002</v>
+      </c>
+      <c r="G5" s="2">
+        <v>39517896410.847198</v>
+      </c>
+      <c r="H5" s="2">
+        <v>280383895.35891002</v>
+      </c>
+      <c r="I5" s="2">
+        <v>224006778.628158</v>
+      </c>
+      <c r="J5" s="2">
+        <v>108838164.16963699</v>
+      </c>
+      <c r="K5" s="2">
+        <v>613228838.15670705</v>
+      </c>
+      <c r="L5" s="45">
+        <v>0.70951118562563098</v>
+      </c>
+      <c r="M5" s="45">
+        <v>0.56684894433467703</v>
+      </c>
+      <c r="N5" s="45">
+        <v>0.27541487289227901</v>
+      </c>
+      <c r="O5" s="45">
+        <v>1.5517750028525801</v>
+      </c>
+      <c r="P5" s="32">
+        <v>0.507675239353365</v>
+      </c>
+      <c r="Q5" s="32">
+        <v>0.40559638709368001</v>
+      </c>
+      <c r="R5" s="32">
+        <v>0.19706709964519101</v>
+      </c>
+      <c r="S5" s="32">
+        <v>1.1103387260922299</v>
+      </c>
+      <c r="T5" s="32">
+        <v>0.62595822013466695</v>
+      </c>
+      <c r="U5" s="32">
+        <v>0.50009607102680598</v>
+      </c>
+      <c r="V5" s="32">
+        <v>0.24298165712813899</v>
+      </c>
+      <c r="W5" s="32">
+        <v>1.3690359482896099</v>
+      </c>
+      <c r="X5" s="2">
+        <v>33646067.443069302</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>26880813.435378999</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>13060579.7003564</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>73587460.578804806</v>
+      </c>
+      <c r="AB5" s="33">
+        <f t="shared" si="0"/>
+        <v>3.5712203352647173E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2747628.8515828899</v>
+      </c>
+      <c r="C6" s="2">
+        <v>62300009849.796898</v>
+      </c>
+      <c r="D6" s="2">
+        <v>49501029635.587097</v>
+      </c>
+      <c r="E6" s="2">
+        <v>23802239836.017101</v>
+      </c>
+      <c r="F6" s="2">
+        <v>19654031599.593601</v>
+      </c>
+      <c r="G6" s="2">
+        <v>43456271435.610802</v>
+      </c>
+      <c r="H6" s="2">
+        <v>369224851.507433</v>
+      </c>
+      <c r="I6" s="2">
+        <v>320476744.428626</v>
+      </c>
+      <c r="J6" s="2">
+        <v>140251683.978917</v>
+      </c>
+      <c r="K6" s="2">
+        <v>829953279.91497695</v>
+      </c>
+      <c r="L6" s="45">
+        <v>0.84964687330461297</v>
+      </c>
+      <c r="M6" s="45">
+        <v>0.737469492529926</v>
+      </c>
+      <c r="N6" s="45">
+        <v>0.32274210222275501</v>
+      </c>
+      <c r="O6" s="45">
+        <v>1.9098584680572901</v>
+      </c>
+      <c r="P6" s="32">
+        <v>0.59265616875120997</v>
+      </c>
+      <c r="Q6" s="32">
+        <v>0.51440881823499596</v>
+      </c>
+      <c r="R6" s="32">
+        <v>0.22512305265610499</v>
+      </c>
+      <c r="S6" s="32">
+        <v>1.33218803964231</v>
+      </c>
+      <c r="T6" s="32">
+        <v>0.74589327580772302</v>
+      </c>
+      <c r="U6" s="32">
+        <v>0.64741429983959398</v>
+      </c>
+      <c r="V6" s="32">
+        <v>0.28333084182573798</v>
+      </c>
+      <c r="W6" s="32">
+        <v>1.67663841747305</v>
+      </c>
+      <c r="X6" s="2">
+        <v>44306982.180891901</v>
+      </c>
+      <c r="Y6" s="2">
+        <v>38457209.331435204</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>16830202.077470001</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>99594393.589797303</v>
+      </c>
+      <c r="AB6" s="33">
+        <f t="shared" si="0"/>
+        <v>4.8333441712579743E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2748336.9317767601</v>
+      </c>
+      <c r="C7" s="2">
+        <v>70697712578.309692</v>
+      </c>
+      <c r="D7" s="2">
+        <v>54853430904.834999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>26514380477.310398</v>
+      </c>
+      <c r="F7" s="2">
+        <v>21273415620.797298</v>
+      </c>
+      <c r="G7" s="2">
+        <v>47787796098.107697</v>
+      </c>
+      <c r="H7" s="2">
+        <v>565914052.89645898</v>
+      </c>
+      <c r="I7" s="2">
+        <v>377309296.38787502</v>
+      </c>
+      <c r="J7" s="2">
+        <v>193414713.33456701</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1136638062.6189001</v>
+      </c>
+      <c r="L7" s="45">
+        <v>1.1842229587961</v>
+      </c>
+      <c r="M7" s="45">
+        <v>0.78955157424139</v>
+      </c>
+      <c r="N7" s="45">
+        <v>0.40473662551311101</v>
+      </c>
+      <c r="O7" s="45">
+        <v>2.3785111585505998</v>
+      </c>
+      <c r="P7" s="32">
+        <v>0.80047010328603296</v>
+      </c>
+      <c r="Q7" s="32">
+        <v>0.533693782482624</v>
+      </c>
+      <c r="R7" s="32">
+        <v>0.27357987448367199</v>
+      </c>
+      <c r="S7" s="32">
+        <v>1.6077437602523299</v>
+      </c>
+      <c r="T7" s="32">
+        <v>1.0316839686441099</v>
+      </c>
+      <c r="U7" s="32">
+        <v>0.68784994878892403</v>
+      </c>
+      <c r="V7" s="32">
+        <v>0.35260276366326399</v>
+      </c>
+      <c r="W7" s="32">
+        <v>2.0721366810962998</v>
+      </c>
+      <c r="X7" s="2">
+        <v>67909686.347575098</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>45277115.566545002</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>23209765.6001481</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>136396567.51426801</v>
+      </c>
+      <c r="AB7" s="33">
+        <f t="shared" si="0"/>
+        <v>6.6193641108952692E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2747846.3569293302</v>
+      </c>
+      <c r="C8" s="2">
+        <v>80541995781.497406</v>
+      </c>
+      <c r="D8" s="2">
+        <v>60962714759.237099</v>
+      </c>
+      <c r="E8" s="2">
+        <v>29745178079.321999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>23156145640.561298</v>
+      </c>
+      <c r="G8" s="2">
+        <v>52901323719.883301</v>
+      </c>
+      <c r="H8" s="2">
+        <v>769257383.36976194</v>
+      </c>
+      <c r="I8" s="2">
+        <v>477587225.23764098</v>
+      </c>
+      <c r="J8" s="2">
+        <v>319343320.21289903</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1566187928.8203001</v>
+      </c>
+      <c r="L8" s="45">
+        <v>1.4541363604491999</v>
+      </c>
+      <c r="M8" s="45">
+        <v>0.90278879932476397</v>
+      </c>
+      <c r="N8" s="45">
+        <v>0.60365846779911803</v>
+      </c>
+      <c r="O8" s="45">
+        <v>2.9605836275730799</v>
+      </c>
+      <c r="P8" s="32">
+        <v>0.95510097050075904</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>0.59296671333212103</v>
+      </c>
+      <c r="R8" s="32">
+        <v>0.39649293156236898</v>
+      </c>
+      <c r="S8" s="32">
+        <v>1.9445606153952499</v>
+      </c>
+      <c r="T8" s="32">
+        <v>1.2618489619562101</v>
+      </c>
+      <c r="U8" s="32">
+        <v>0.78340872305932996</v>
+      </c>
+      <c r="V8" s="32">
+        <v>0.52383382445171001</v>
+      </c>
+      <c r="W8" s="32">
+        <v>2.56909150946725</v>
+      </c>
+      <c r="X8" s="2">
+        <v>92310886.004371494</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>57310467.028516904</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>38321198.425547898</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>187942551.45843601</v>
+      </c>
+      <c r="AB8" s="33">
+        <f t="shared" si="0"/>
+        <v>9.1209053329287151E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2747984.4327531499</v>
+      </c>
+      <c r="C9" s="2">
+        <v>95316514865.332199</v>
+      </c>
+      <c r="D9" s="2">
+        <v>69592985603.748001</v>
+      </c>
+      <c r="E9" s="2">
+        <v>33990731017.6814</v>
+      </c>
+      <c r="F9" s="2">
+        <v>25837312021.747002</v>
+      </c>
+      <c r="G9" s="2">
+        <v>59828043039.428398</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1207378903.46699</v>
+      </c>
+      <c r="I9" s="2">
+        <v>672596958.40017295</v>
+      </c>
+      <c r="J9" s="2">
+        <v>501199512.93965501</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2381175374.8068299</v>
+      </c>
+      <c r="L9" s="45">
+        <v>2.0180818929198399</v>
+      </c>
+      <c r="M9" s="45">
+        <v>1.12421687929339</v>
+      </c>
+      <c r="N9" s="45">
+        <v>0.837733423119573</v>
+      </c>
+      <c r="O9" s="45">
+        <v>3.9800321953328202</v>
+      </c>
+      <c r="P9" s="32">
+        <v>1.26670483616909</v>
+      </c>
+      <c r="Q9" s="32">
+        <v>0.70564577329589795</v>
+      </c>
+      <c r="R9" s="32">
+        <v>0.52582651983003603</v>
+      </c>
+      <c r="S9" s="32">
+        <v>2.4981771292950299</v>
+      </c>
+      <c r="T9" s="32">
+        <v>1.73491465122883</v>
+      </c>
+      <c r="U9" s="32">
+        <v>0.966472342816039</v>
+      </c>
+      <c r="V9" s="32">
+        <v>0.72018682427767899</v>
+      </c>
+      <c r="W9" s="32">
+        <v>3.4215738183225501</v>
+      </c>
+      <c r="X9" s="2">
+        <v>144885468.41603899</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>80711635.008020699</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>60143941.552758701</v>
+      </c>
+      <c r="AA9" s="2">
+        <v>285741044.97681898</v>
+      </c>
+      <c r="AB9" s="33">
+        <f t="shared" si="0"/>
+        <v>0.13867093964306768</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2748042.5822946099</v>
+      </c>
+      <c r="C10" s="2">
+        <v>117372854152.933</v>
+      </c>
+      <c r="D10" s="2">
+        <v>82061193028.969299</v>
+      </c>
+      <c r="E10" s="2">
+        <v>40157035542.102303</v>
+      </c>
+      <c r="F10" s="2">
+        <v>29129990531.2584</v>
+      </c>
+      <c r="G10" s="2">
+        <v>69287026073.360703</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1874891792.81111</v>
+      </c>
+      <c r="I10" s="2">
+        <v>875936426.44145405</v>
+      </c>
+      <c r="J10" s="2">
+        <v>610654839.69481397</v>
+      </c>
+      <c r="K10" s="2">
+        <v>3361483058.9473701</v>
+      </c>
+      <c r="L10" s="45">
+        <v>2.7059781593540801</v>
+      </c>
+      <c r="M10" s="45">
+        <v>1.26421420586592</v>
+      </c>
+      <c r="N10" s="45">
+        <v>0.88134081414932797</v>
+      </c>
+      <c r="O10" s="45">
+        <v>4.8515331793693299</v>
+      </c>
+      <c r="P10" s="32">
+        <v>1.59738110344337</v>
+      </c>
+      <c r="Q10" s="32">
+        <v>0.746285359389944</v>
+      </c>
+      <c r="R10" s="32">
+        <v>0.52026922588007296</v>
+      </c>
+      <c r="S10" s="32">
+        <v>2.86393568871339</v>
+      </c>
+      <c r="T10" s="32">
+        <v>2.2847483976369101</v>
+      </c>
+      <c r="U10" s="32">
+        <v>1.06741858619119</v>
+      </c>
+      <c r="V10" s="32">
+        <v>0.74414570048870698</v>
+      </c>
+      <c r="W10" s="32">
+        <v>4.0963126843168096</v>
+      </c>
+      <c r="X10" s="2">
+        <v>224987015.13733301</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>105112371.17297401</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>73278580.763377696</v>
+      </c>
+      <c r="AA10" s="2">
+        <v>403377967.07368499</v>
+      </c>
+      <c r="AB10" s="33">
+        <f t="shared" si="0"/>
+        <v>0.19576047161847621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2748063.5193039002</v>
+      </c>
+      <c r="C11" s="2">
+        <v>205068163103.01001</v>
+      </c>
+      <c r="D11" s="2">
+        <v>124958992792.82401</v>
+      </c>
+      <c r="E11" s="2">
+        <v>60239542360.468002</v>
+      </c>
+      <c r="F11" s="2">
+        <v>40132550257.43</v>
+      </c>
+      <c r="G11" s="2">
+        <v>100372092617.89799</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3388003188.5553999</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1423730211.27795</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1597945068.6734099</v>
+      </c>
+      <c r="K11" s="2">
+        <v>6409678468.5067701</v>
+      </c>
+      <c r="L11" s="45">
+        <v>3.3754434127950601</v>
+      </c>
+      <c r="M11" s="45">
+        <v>1.41845225514814</v>
+      </c>
+      <c r="N11" s="45">
+        <v>1.59202127503364</v>
+      </c>
+      <c r="O11" s="45">
+        <v>6.3859169429768396</v>
+      </c>
+      <c r="P11" s="32">
+        <v>1.6521351424274999</v>
+      </c>
+      <c r="Q11" s="32">
+        <v>0.69427169470610794</v>
+      </c>
+      <c r="R11" s="32">
+        <v>0.77922630431459206</v>
+      </c>
+      <c r="S11" s="32">
+        <v>3.1256331414481999</v>
+      </c>
+      <c r="T11" s="32">
+        <v>2.7112920109499599</v>
+      </c>
+      <c r="U11" s="32">
+        <v>1.13935794412045</v>
+      </c>
+      <c r="V11" s="32">
+        <v>1.27877556705559</v>
+      </c>
+      <c r="W11" s="32">
+        <v>5.1294255221260103</v>
+      </c>
+      <c r="X11" s="2">
+        <v>406560382.626647</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>170847625.35335499</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>191753408.24080899</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>769161416.22081196</v>
+      </c>
+      <c r="AB11" s="33">
+        <f t="shared" si="0"/>
+        <v>0.37327621704885128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28">
+      <c r="A12" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="5">
+        <f t="shared" ref="B12:Z12" si="1">SUM(B2:B11)</f>
+        <v>27479695.00677811</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="1"/>
+        <v>808884408912.44861</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="1"/>
+        <v>590923379472.91711</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>283018492377.6701</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="1"/>
+        <v>223463602629.93637</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="1"/>
+        <v>506482095007.60669</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="1"/>
+        <v>8849912765.443203</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="1"/>
+        <v>4704838464.2325029</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="1"/>
+        <v>3616657437.0273142</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="1"/>
+        <v>17171408666.703037</v>
+      </c>
+      <c r="L12" s="46">
+        <f t="shared" si="1"/>
+        <v>13.528974904142064</v>
+      </c>
+      <c r="M12" s="46">
+        <f t="shared" si="1"/>
+        <v>7.8456240443426202</v>
+      </c>
+      <c r="N12" s="46">
+        <f t="shared" si="1"/>
+        <v>5.3764639875078064</v>
+      </c>
+      <c r="O12" s="46">
+        <f t="shared" si="1"/>
+        <v>26.751062935992486</v>
+      </c>
+      <c r="P12" s="44">
+        <f t="shared" si="1"/>
+        <v>8.3075460941495365</v>
+      </c>
+      <c r="Q12" s="44">
+        <f t="shared" si="1"/>
+        <v>4.9846612132532302</v>
+      </c>
+      <c r="R12" s="44">
+        <f t="shared" si="1"/>
+        <v>3.2677987887765623</v>
+      </c>
+      <c r="S12" s="44">
+        <f t="shared" si="1"/>
+        <v>16.560006096179336</v>
+      </c>
+      <c r="T12" s="44">
+        <f t="shared" si="1"/>
+        <v>11.498474193390338</v>
+      </c>
+      <c r="U12" s="44">
+        <f t="shared" si="1"/>
+        <v>6.7244508142303321</v>
+      </c>
+      <c r="V12" s="44">
+        <f t="shared" si="1"/>
+        <v>4.5567545313934188</v>
+      </c>
+      <c r="W12" s="44">
+        <f t="shared" si="1"/>
+        <v>22.779679539014101</v>
+      </c>
+      <c r="X12" s="5">
+        <f t="shared" si="1"/>
+        <v>1061989531.8531835</v>
+      </c>
+      <c r="Y12" s="5">
+        <f t="shared" si="1"/>
+        <v>564580615.70790088</v>
+      </c>
+      <c r="Z12" s="5">
+        <f t="shared" si="1"/>
+        <v>433998892.4432776</v>
+      </c>
+      <c r="AA12" s="5">
+        <f>SUM(AA2:AA11)</f>
+        <v>2060569040.0043635</v>
+      </c>
+      <c r="AB12" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28">
+      <c r="K14" s="28">
+        <f>K12/G12</f>
+        <v>3.3903288657114609E-2</v>
+      </c>
+      <c r="L14" s="33">
+        <f>H12/G12</f>
+        <v>1.7473298370617205E-2</v>
+      </c>
+      <c r="X14" s="3">
+        <f>H12*12%</f>
+        <v>1061989531.8531843</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61A1F9D-EB5B-1C46-BEE0-9C566D64DA42}">
   <dimension ref="A1:U24"/>
   <sheetViews>
@@ -8657,7 +10309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA719825-5205-FE4C-B220-F0E805A976AA}">
   <dimension ref="A1:O24"/>
   <sheetViews>
@@ -9454,7 +11106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2835AA48-B8D0-BB4F-9D44-004653D39453}">
   <dimension ref="A1:R11"/>
   <sheetViews>
@@ -10095,7 +11747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79482C87-9E54-3145-A88B-A07A29DD7EB7}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -10526,479 +12178,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EEC793-A1C4-FF48-AB6B-B60CEDF4D66E}">
-  <dimension ref="A1:K15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="6" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2747642.50515944</v>
-      </c>
-      <c r="C2" s="2">
-        <v>12730887016.797501</v>
-      </c>
-      <c r="D2" s="2">
-        <v>13799492511.298201</v>
-      </c>
-      <c r="E2" s="2">
-        <v>26530379528.095699</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1527706442.0157001</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1655939101.3557799</v>
-      </c>
-      <c r="H2" s="1">
-        <v>5.7081655079756999</v>
-      </c>
-      <c r="I2" s="1">
-        <v>6.2918344920242903</v>
-      </c>
-      <c r="J2" s="1">
-        <v>5.7583286375449596</v>
-      </c>
-      <c r="K2" s="1">
-        <v>6.2416713624550297</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2748295.6540946802</v>
-      </c>
-      <c r="C3" s="2">
-        <v>16171881744.9347</v>
-      </c>
-      <c r="D3" s="2">
-        <v>15540656739.6842</v>
-      </c>
-      <c r="E3" s="2">
-        <v>31712538484.6189</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1940625809.3921599</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1864878808.7621</v>
-      </c>
-      <c r="H3" s="1">
-        <v>6.0303049401519999</v>
-      </c>
-      <c r="I3" s="1">
-        <v>5.9696950598479903</v>
-      </c>
-      <c r="J3" s="1">
-        <v>6.11942752653938</v>
-      </c>
-      <c r="K3" s="1">
-        <v>5.8805724734606102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2747874.69444041</v>
-      </c>
-      <c r="C4" s="2">
-        <v>18492395560.589802</v>
-      </c>
-      <c r="D4" s="2">
-        <v>16596332039.166201</v>
-      </c>
-      <c r="E4" s="2">
-        <v>35088727599.755997</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2219087467.2707801</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1991559844.69994</v>
-      </c>
-      <c r="H4" s="1">
-        <v>6.1898610711613902</v>
-      </c>
-      <c r="I4" s="1">
-        <v>5.8101389288386098</v>
-      </c>
-      <c r="J4" s="1">
-        <v>6.3242175452557801</v>
-      </c>
-      <c r="K4" s="1">
-        <v>5.6757824547442102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>2747979.4784429399</v>
-      </c>
-      <c r="C5" s="2">
-        <v>21174220742.446899</v>
-      </c>
-      <c r="D5" s="2">
-        <v>18343675668.4002</v>
-      </c>
-      <c r="E5" s="2">
-        <v>39517896410.847198</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2540906489.0936298</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2201241080.2080202</v>
-      </c>
-      <c r="H5" s="1">
-        <v>6.2902942340410304</v>
-      </c>
-      <c r="I5" s="1">
-        <v>5.7097057659589598</v>
-      </c>
-      <c r="J5" s="1">
-        <v>6.4297615001495503</v>
-      </c>
-      <c r="K5" s="1">
-        <v>5.57023849985044</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2747628.8515828899</v>
-      </c>
-      <c r="C6" s="2">
-        <v>23802239836.017101</v>
-      </c>
-      <c r="D6" s="2">
-        <v>19654031599.593601</v>
-      </c>
-      <c r="E6" s="2">
-        <v>43456271435.610802</v>
-      </c>
-      <c r="F6" s="2">
-        <v>2856268780.3220501</v>
-      </c>
-      <c r="G6" s="2">
-        <v>2358483791.9512401</v>
-      </c>
-      <c r="H6" s="1">
-        <v>6.4047799708266</v>
-      </c>
-      <c r="I6" s="1">
-        <v>5.5952200291733902</v>
-      </c>
-      <c r="J6" s="1">
-        <v>6.5727424050960996</v>
-      </c>
-      <c r="K6" s="1">
-        <v>5.4272575949038897</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2748336.9317767601</v>
-      </c>
-      <c r="C7" s="2">
-        <v>26514380477.310398</v>
-      </c>
-      <c r="D7" s="2">
-        <v>21273415620.797298</v>
-      </c>
-      <c r="E7" s="2">
-        <v>47787796098.107697</v>
-      </c>
-      <c r="F7" s="2">
-        <v>3181725657.2772498</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2552809874.4956799</v>
-      </c>
-      <c r="H7" s="1">
-        <v>6.4988720176579404</v>
-      </c>
-      <c r="I7" s="1">
-        <v>5.5011279823420498</v>
-      </c>
-      <c r="J7" s="1">
-        <v>6.6580297001878996</v>
-      </c>
-      <c r="K7" s="1">
-        <v>5.3419702998121004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>2747846.3569293302</v>
-      </c>
-      <c r="C8" s="2">
-        <v>29745178079.321999</v>
-      </c>
-      <c r="D8" s="2">
-        <v>23156145640.561298</v>
-      </c>
-      <c r="E8" s="2">
-        <v>52901323719.883301</v>
-      </c>
-      <c r="F8" s="2">
-        <v>3569421369.51863</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2778737476.8673501</v>
-      </c>
-      <c r="H8" s="1">
-        <v>6.62365764514223</v>
-      </c>
-      <c r="I8" s="1">
-        <v>5.3763423548577602</v>
-      </c>
-      <c r="J8" s="1">
-        <v>6.7473195726046598</v>
-      </c>
-      <c r="K8" s="1">
-        <v>5.2526804273953296</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2747984.4327531499</v>
-      </c>
-      <c r="C9" s="2">
-        <v>33990731017.6814</v>
-      </c>
-      <c r="D9" s="2">
-        <v>25837312021.747002</v>
-      </c>
-      <c r="E9" s="2">
-        <v>59828043039.428398</v>
-      </c>
-      <c r="F9" s="2">
-        <v>4078887722.1217699</v>
-      </c>
-      <c r="G9" s="2">
-        <v>3100477442.6096401</v>
-      </c>
-      <c r="H9" s="1">
-        <v>6.7137976077127703</v>
-      </c>
-      <c r="I9" s="1">
-        <v>5.2862023922872199</v>
-      </c>
-      <c r="J9" s="1">
-        <v>6.8176853443688001</v>
-      </c>
-      <c r="K9" s="1">
-        <v>5.1823146556311901</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2">
-        <v>2748042.5822946099</v>
-      </c>
-      <c r="C10" s="2">
-        <v>40157035542.102303</v>
-      </c>
-      <c r="D10" s="2">
-        <v>29129990531.2584</v>
-      </c>
-      <c r="E10" s="2">
-        <v>69287026073.360703</v>
-      </c>
-      <c r="F10" s="2">
-        <v>4818844265.0522804</v>
-      </c>
-      <c r="G10" s="2">
-        <v>3495598863.7510099</v>
-      </c>
-      <c r="H10" s="1">
-        <v>6.8620584936718902</v>
-      </c>
-      <c r="I10" s="1">
-        <v>5.1379415063281</v>
-      </c>
-      <c r="J10" s="1">
-        <v>6.9549012826010399</v>
-      </c>
-      <c r="K10" s="1">
-        <v>5.0450987173989601</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2748063.5193039002</v>
-      </c>
-      <c r="C11" s="2">
-        <v>60239542360.468002</v>
-      </c>
-      <c r="D11" s="2">
-        <v>40132550257.43</v>
-      </c>
-      <c r="E11" s="2">
-        <v>100372092617.89799</v>
-      </c>
-      <c r="F11" s="2">
-        <v>7228745083.2561598</v>
-      </c>
-      <c r="G11" s="2">
-        <v>4815906030.8915997</v>
-      </c>
-      <c r="H11" s="1">
-        <v>7.1193827019703901</v>
-      </c>
-      <c r="I11" s="1">
-        <v>4.8806172980296099</v>
-      </c>
-      <c r="J11" s="1">
-        <v>7.2019471694935504</v>
-      </c>
-      <c r="K11" s="1">
-        <v>4.7980528305064398</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1">
-      <c r="A12" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="5">
-        <f t="shared" ref="B12:G12" si="0">SUM(B2:B11)</f>
-        <v>27479695.00677811</v>
-      </c>
-      <c r="C12" s="5">
-        <f t="shared" si="0"/>
-        <v>283018492377.6701</v>
-      </c>
-      <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>223463602629.93637</v>
-      </c>
-      <c r="E12" s="5">
-        <f t="shared" si="0"/>
-        <v>506482095007.60669</v>
-      </c>
-      <c r="F12" s="5">
-        <f t="shared" si="0"/>
-        <v>33962219085.320412</v>
-      </c>
-      <c r="G12" s="5">
-        <f t="shared" si="0"/>
-        <v>26815632315.592361</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="C13" s="6">
-        <f>C12/E12</f>
-        <v>0.558792690141237</v>
-      </c>
-      <c r="D13" s="6">
-        <f>D12/E12</f>
-        <v>0.44120730985876261</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="C14" s="3">
-        <f>C12*12</f>
-        <v>3396221908532.041</v>
-      </c>
-      <c r="D14" s="3">
-        <f>D12*12</f>
-        <v>2681563231559.2363</v>
-      </c>
-      <c r="E14" s="3">
-        <f>E12*12</f>
-        <v>6077785140091.2803</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="C15" s="3">
-        <f>C14*0.12</f>
-        <v>407546629023.84491</v>
-      </c>
-      <c r="D15" s="3">
-        <f>D14*0.12</f>
-        <v>321787587787.10834</v>
-      </c>
-      <c r="E15" s="3">
-        <f>E14*0.12</f>
-        <v>729334216810.95361</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>